<commit_message>
Work out VGA interface
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2018E2-22E1-411A-9EBE-A89411B57760}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8AFF3B-00A7-4930-B7DA-8A8B9B802D3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>Initialize repo, create documentation</t>
+  </si>
+  <si>
+    <t>VGA Interface</t>
+  </si>
+  <si>
+    <t>Read into subject, take notes</t>
   </si>
 </sst>
 </file>
@@ -381,7 +387,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -432,8 +438,25 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="D3" s="1">
+        <f>C3-B3</f>
+        <v>4.8611111111111049E-2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Crate necessary files for Pattern Generator 1
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8AFF3B-00A7-4930-B7DA-8A8B9B802D3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF3FA38-C6D2-4F40-82DA-E5EBD83AAFDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>Read into subject, take notes</t>
+  </si>
+  <si>
+    <t>Pattern Gen 1</t>
+  </si>
+  <si>
+    <t>Create necessary files</t>
   </si>
 </sst>
 </file>
@@ -384,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -458,6 +464,27 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.57986111111111105</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="D4" s="1">
+        <f>C4-B4</f>
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
First construct of Pattern Generator 1
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF3FA38-C6D2-4F40-82DA-E5EBD83AAFDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9D910E-7ED8-4CFB-9CB7-7A54784296D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -72,14 +72,28 @@
   </si>
   <si>
     <t>Create necessary files</t>
+  </si>
+  <si>
+    <t>3.3.2020</t>
+  </si>
+  <si>
+    <t>Concept of module</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -107,9 +121,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -402,90 +430,133 @@
     <col min="6" max="6" width="42.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
         <v>0.40277777777777773</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="4">
         <f>C2-B2</f>
         <v>1.3888888888888951E-2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>0.46527777777777773</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="4">
         <f>C3-B3</f>
         <v>4.8611111111111049E-2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="4">
         <v>0.57986111111111105</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>0.59027777777777779</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="4">
         <f>C4-B4</f>
         <v>1.0416666666666741E-2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" ref="D5:D6" si="0">C5-B5</f>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
+        <v>1.3888888888888895E-2</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Create source code for Pattern Generator 1
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9D910E-7ED8-4CFB-9CB7-7A54784296D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D44C10A-2D68-4905-9D47-F1C425E19F12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>Concept of module</t>
+  </si>
+  <si>
+    <t>9.3.2020</t>
+  </si>
+  <si>
+    <t>VHDL files</t>
   </si>
 </sst>
 </file>
@@ -121,11 +127,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -137,6 +140,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -418,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -430,37 +440,37 @@
     <col min="6" max="6" width="42.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>0.40277777777777773</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <f>C2-B2</f>
         <v>1.3888888888888951E-2</v>
       </c>
@@ -472,16 +482,16 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>0.46527777777777773</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <f>C3-B3</f>
         <v>4.8611111111111049E-2</v>
       </c>
@@ -493,16 +503,16 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>0.57986111111111105</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>0.59027777777777779</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <f>C4-B4</f>
         <v>1.0416666666666741E-2</v>
       </c>
@@ -514,42 +524,63 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>0.34722222222222227</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>0.3611111111111111</v>
       </c>
-      <c r="D5" s="4">
-        <f t="shared" ref="D5:D6" si="0">C5-B5</f>
+      <c r="D5" s="3">
+        <f t="shared" ref="D5:D7" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>0.375</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>0.3888888888888889</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <f t="shared" si="0"/>
         <v>1.3888888888888895E-2</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.4375</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>2.7777777777777735E-2</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Initial commit for Pattern Generator 2
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F1B7DD-49E6-4712-B429-B7A9643BFBA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B6C454-9684-470C-9570-D4DAB6FE0507}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>Comment files</t>
+  </si>
+  <si>
+    <t>29.3.2020</t>
+  </si>
+  <si>
+    <t>Pattern Gen 2</t>
   </si>
 </sst>
 </file>
@@ -431,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -537,7 +543,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D8" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D9" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -605,6 +611,30 @@
       <c r="F8" s="6" t="s">
         <v>17</v>
       </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Pattern Gen 2 architecture and testbench
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B6C454-9684-470C-9570-D4DAB6FE0507}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2084CA34-FFD9-4385-8CE6-B1D1BE5FE053}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="338" yWindow="1755" windowWidth="13680" windowHeight="9532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Pattern Gen 2</t>
+  </si>
+  <si>
+    <t>RTL and TB</t>
   </si>
 </sst>
 </file>
@@ -440,7 +443,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -543,7 +546,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D9" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D10" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -634,7 +637,25 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Create files for IO Control Unit
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2084CA34-FFD9-4385-8CE6-B1D1BE5FE053}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B587926-579A-459C-9F8B-512002FC4019}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="338" yWindow="1755" windowWidth="13680" windowHeight="9532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>RTL and TB</t>
+  </si>
+  <si>
+    <t>30.3.2020</t>
+  </si>
+  <si>
+    <t>IO Control</t>
   </si>
 </sst>
 </file>
@@ -440,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -546,7 +552,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D10" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D11" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -656,6 +662,31 @@
       <c r="F10" s="6" t="s">
         <v>20</v>
       </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.43402777777777773</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="2"/>
+      <c r="B12" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
IO Control architecture and testbench
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B587926-579A-459C-9F8B-512002FC4019}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDF1C62-2A5F-4602-B0D9-F99194D37A10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="338" yWindow="1755" windowWidth="13680" windowHeight="9532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -168,7 +168,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -449,16 +449,16 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="25.1328125" customWidth="1"/>
-    <col min="6" max="6" width="42.59765625" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -478,7 +478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -499,7 +499,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -520,7 +520,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -541,7 +541,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -552,7 +552,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D11" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D12" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -562,7 +562,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -579,7 +579,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -600,7 +600,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -621,7 +621,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -642,7 +642,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -663,7 +663,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -684,9 +684,26 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="2"/>
-      <c r="B12" s="5"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>3.819444444444442E-2</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Source MUX architecture and testbench
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDF1C62-2A5F-4602-B0D9-F99194D37A10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AB4562-F08A-4181-B4D1-8ADB214F93AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>IO Control</t>
+  </si>
+  <si>
+    <t>Source MUX</t>
   </si>
 </sst>
 </file>
@@ -446,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +555,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D12" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D14" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -702,6 +705,48 @@
         <v>22</v>
       </c>
       <c r="F12" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.49652777777777773</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444753E-3</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="5">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>1.736111111111116E-2</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add initial files for VGA Control
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AB4562-F08A-4181-B4D1-8ADB214F93AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CF97F6-24E0-4CE3-A411-A2D6982AA53D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Source MUX</t>
+  </si>
+  <si>
+    <t>VGA Control</t>
   </si>
 </sst>
 </file>
@@ -449,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +558,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D14" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D15" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -748,6 +751,27 @@
       </c>
       <c r="F14" s="6" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.53125</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
VGA Control architecture and testbench
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CF97F6-24E0-4CE3-A411-A2D6982AA53D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95068DF-572F-4026-8459-0B4A07CCD979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -452,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +558,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D15" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D16" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -772,6 +772,27 @@
       </c>
       <c r="F15" s="6" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0.6875</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>0.10416666666666663</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve VGA control code
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95068DF-572F-4026-8459-0B4A07CCD979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A987ADA-0F67-4F5D-BE7E-AD67F77215A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>VGA Control</t>
+  </si>
+  <si>
+    <t>31.3.2020</t>
+  </si>
+  <si>
+    <t>Improve RTL</t>
+  </si>
+  <si>
+    <t>Improve TB</t>
   </si>
 </sst>
 </file>
@@ -452,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +567,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D16" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D18" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -794,6 +803,51 @@
       <c r="F16" s="6" t="s">
         <v>20</v>
       </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333315E-2</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Add initial files for VGA Top
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9B17CD-6015-4143-B089-65236D4612DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5934642-1CC6-4C7E-9FF2-9FDE6BDCECF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>1.4.2020</t>
+  </si>
+  <si>
+    <t>VGA Top</t>
   </si>
 </sst>
 </file>
@@ -467,7 +470,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,7 +573,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D19" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D20" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -868,6 +871,27 @@
       </c>
       <c r="F19" s="6" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="4:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Improve source MUX code
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5934642-1CC6-4C7E-9FF2-9FDE6BDCECF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853704E6-A09E-4B1A-AA8B-D7ED07E4B59F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -123,6 +123,21 @@
   </si>
   <si>
     <t>VGA Top</t>
+  </si>
+  <si>
+    <t>VGA Debounce</t>
+  </si>
+  <si>
+    <t>Revision</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Change IO Control to IO Debounce</t>
+  </si>
+  <si>
+    <t>Improve Code</t>
   </si>
 </sst>
 </file>
@@ -467,19 +482,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="25.140625" customWidth="1"/>
     <col min="6" max="6" width="42.5703125" customWidth="1"/>
+    <col min="7" max="7" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -493,13 +509,16 @@
         <v>4</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -520,7 +539,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -541,7 +560,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -562,7 +581,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -573,7 +592,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D20" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D22" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -583,7 +602,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -600,7 +619,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -621,7 +640,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -642,7 +661,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -663,7 +682,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -684,7 +703,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -705,7 +724,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -726,7 +745,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -747,7 +766,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -768,7 +787,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -789,7 +808,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -810,7 +829,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>25</v>
       </c>
@@ -831,7 +850,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
@@ -852,7 +871,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>28</v>
       </c>
@@ -873,7 +892,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
@@ -892,6 +911,51 @@
       </c>
       <c r="F20" s="6" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="5">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="0"/>
+        <v>5.2083333333333315E-2</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0.53125</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="0"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="4:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Architecture and Testbench of VGA top
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853704E6-A09E-4B1A-AA8B-D7ED07E4B59F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50A422A-B623-4F5A-9853-B19BCB40527A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Pattern Gen 2</t>
   </si>
   <si>
-    <t>RTL and TB</t>
-  </si>
-  <si>
     <t>30.3.2020</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>31.3.2020</t>
   </si>
   <si>
-    <t>Improve RTL</t>
-  </si>
-  <si>
     <t>Improve TB</t>
   </si>
   <si>
@@ -138,6 +132,12 @@
   </si>
   <si>
     <t>Improve Code</t>
+  </si>
+  <si>
+    <t>Arch and TB</t>
+  </si>
+  <si>
+    <t>Improve Arch</t>
   </si>
 </sst>
 </file>
@@ -485,7 +485,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +509,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>6</v>
@@ -592,7 +592,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D22" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D24" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -700,12 +700,12 @@
         <v>19</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="5">
         <v>0.42708333333333331</v>
@@ -718,7 +718,7 @@
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>12</v>
@@ -726,7 +726,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="5">
         <v>0.4513888888888889</v>
@@ -739,15 +739,15 @@
         <v>3.819444444444442E-2</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="5">
         <v>0.49652777777777773</v>
@@ -760,7 +760,7 @@
         <v>6.9444444444444753E-3</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>12</v>
@@ -768,7 +768,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="5">
         <v>0.50347222222222221</v>
@@ -781,15 +781,15 @@
         <v>1.736111111111116E-2</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="5">
         <v>0.52083333333333337</v>
@@ -802,7 +802,7 @@
         <v>1.041666666666663E-2</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>12</v>
@@ -810,7 +810,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="5">
         <v>0.58333333333333337</v>
@@ -823,15 +823,15 @@
         <v>0.10416666666666663</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="5">
         <v>0.45833333333333331</v>
@@ -844,15 +844,15 @@
         <v>8.3333333333333315E-2</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="5">
         <v>0.58333333333333337</v>
@@ -865,15 +865,15 @@
         <v>3.125E-2</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B19" s="5">
         <v>0.41666666666666669</v>
@@ -886,15 +886,15 @@
         <v>2.0833333333333315E-2</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B20" s="5">
         <v>0.4375</v>
@@ -907,7 +907,7 @@
         <v>1.0416666666666685E-2</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>12</v>
@@ -915,7 +915,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B21" s="5">
         <v>0.44791666666666669</v>
@@ -928,18 +928,18 @@
         <v>5.2083333333333315E-2</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" t="s">
         <v>31</v>
-      </c>
-      <c r="G21" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B22" s="5">
         <v>0.5</v>
@@ -952,10 +952,52 @@
         <v>3.125E-2</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="5">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="0"/>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0.74305555555555547</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="0"/>
+        <v>3.4722222222222099E-2</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="4:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add Pattern Gen 2 to VGA Top testbench
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50A422A-B623-4F5A-9853-B19BCB40527A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24090F7-3A43-4FEF-A56A-41F425834A49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>Improve Arch</t>
+  </si>
+  <si>
+    <t>Add VGA Monitor simulation model</t>
+  </si>
+  <si>
+    <t>Add Pattern Generator 2</t>
   </si>
 </sst>
 </file>
@@ -204,7 +210,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -485,17 +491,17 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="5" max="5" width="25.140625" customWidth="1"/>
-    <col min="6" max="6" width="42.5703125" customWidth="1"/>
-    <col min="7" max="7" width="36.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25.1328125" customWidth="1"/>
+    <col min="6" max="6" width="42.59765625" customWidth="1"/>
+    <col min="7" max="7" width="36.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -518,7 +524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -539,7 +545,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -560,7 +566,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -581,7 +587,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -592,7 +598,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D24" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D26" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -602,7 +608,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -619,7 +625,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -640,7 +646,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -661,7 +667,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -682,7 +688,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -703,7 +709,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -724,7 +730,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -745,7 +751,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -766,7 +772,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -787,7 +793,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -808,7 +814,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -829,7 +835,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
@@ -850,7 +856,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -871,7 +877,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
@@ -892,7 +898,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
@@ -913,7 +919,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
@@ -937,7 +943,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -958,7 +964,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
@@ -979,7 +985,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
@@ -1000,7 +1006,55 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="5">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0.84375</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="0"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="5">
+        <v>0.84375</v>
+      </c>
+      <c r="C26" s="5">
+        <v>0.86111111111111116</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="0"/>
+        <v>1.736111111111116E-2</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D38" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commenting Pattern Gen 1
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F025AA81-3B84-48E2-B889-94A65C575D8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1155E327-7244-45DD-9307-930D662C192D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -213,7 +213,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -494,17 +494,17 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="25.1328125" customWidth="1"/>
-    <col min="6" max="6" width="42.59765625" customWidth="1"/>
-    <col min="7" max="7" width="36.265625" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="42.5703125" customWidth="1"/>
+    <col min="7" max="7" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -527,7 +527,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -548,7 +548,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -569,7 +569,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -590,7 +590,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -601,7 +601,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D27" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D28" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -611,7 +611,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -628,7 +628,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -649,7 +649,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -670,7 +670,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -691,7 +691,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -712,7 +712,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -733,7 +733,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -754,7 +754,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -775,7 +775,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -796,7 +796,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -817,7 +817,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -838,7 +838,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
@@ -859,7 +859,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -880,7 +880,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
@@ -901,7 +901,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
@@ -922,7 +922,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
@@ -946,7 +946,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -967,7 +967,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
@@ -988,7 +988,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
@@ -1078,10 +1078,28 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="D28" s="3"/>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C28" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Comment Pattern Gen 2
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1155E327-7244-45DD-9307-930D662C192D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D88AE20-B595-42F2-B0BC-F3962B8B7E86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -494,7 +494,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,7 +601,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D28" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D30" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1096,6 +1096,48 @@
         <v>11</v>
       </c>
       <c r="F28" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="5">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0.53125</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="0"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="5">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="C30" s="5">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="6" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add PLL IP Core
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7C06B6-45FD-4691-AB86-07BC1166558A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF7533E-8624-4715-BFAD-142F999770D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -150,6 +150,18 @@
   </si>
   <si>
     <t>2.4.2020</t>
+  </si>
+  <si>
+    <t>3.4.2020</t>
+  </si>
+  <si>
+    <t>Clk PLL</t>
+  </si>
+  <si>
+    <t>IP Core</t>
+  </si>
+  <si>
+    <t>Testbench</t>
   </si>
 </sst>
 </file>
@@ -497,7 +509,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +616,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D33" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D35" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1186,7 +1198,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>38</v>
       </c>
@@ -1207,10 +1219,55 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="5">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C34" s="5">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="0"/>
+        <v>3.4722222222222265E-2</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="5">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="C35" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D35" s="3">
+        <f t="shared" si="0"/>
+        <v>2.7777777777777735E-2</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D37" s="5"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D38" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create PLL and ROM 1 IP cores
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF7533E-8624-4715-BFAD-142F999770D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDB5013-2C2D-43C9-BB23-6435FBDF5F29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -162,6 +162,18 @@
   </si>
   <si>
     <t>Testbench</t>
+  </si>
+  <si>
+    <t>Mem Ctrl 1</t>
+  </si>
+  <si>
+    <t>ROM 1</t>
+  </si>
+  <si>
+    <t>4.4.2020</t>
+  </si>
+  <si>
+    <t>Add VGA PLL</t>
   </si>
 </sst>
 </file>
@@ -508,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,7 +628,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D35" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D37" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1264,11 +1276,65 @@
         <v>42</v>
       </c>
     </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="5">
+        <v>0.5625</v>
+      </c>
+      <c r="C36" s="5">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D36" s="3">
+        <f t="shared" si="0"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D37" s="5"/>
+      <c r="A37" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="5">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C37" s="5">
+        <v>0.625</v>
+      </c>
+      <c r="D37" s="5">
+        <f t="shared" si="0"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="5">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="D38" s="5"/>
+      <c r="E38" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G38" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Add ROM 1 testbench
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDB5013-2C2D-43C9-BB23-6435FBDF5F29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3197B847-EE90-4777-A935-BD37A7DE6184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -518,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,7 +628,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D37" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D39" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1325,7 +1325,13 @@
       <c r="B38" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D38" s="5"/>
+      <c r="C38" s="5">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D38" s="5">
+        <f t="shared" si="0"/>
+        <v>1.041666666666663E-2</v>
+      </c>
       <c r="E38" s="6" t="s">
         <v>27</v>
       </c>
@@ -1334,6 +1340,27 @@
       </c>
       <c r="G38" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="C39" s="5">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Memory Control 1 architecture and testbench
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3197B847-EE90-4777-A935-BD37A7DE6184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98D348E-3C54-41E3-A05E-AAB2457CF5AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -521,7 +521,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add Memory Control 1 to VGA Top
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98D348E-3C54-41E3-A05E-AAB2457CF5AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C406858-EFF7-4B60-8F01-E7144E49D0AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t>Add VGA PLL</t>
+  </si>
+  <si>
+    <t>Arch</t>
+  </si>
+  <si>
+    <t>Add Memory Control 1</t>
   </si>
 </sst>
 </file>
@@ -518,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,7 +634,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D39" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D40" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1361,6 +1367,30 @@
       </c>
       <c r="F39" s="6" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="5">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="C40" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G40" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add ROM 1 to VGA Top unit
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C406858-EFF7-4B60-8F01-E7144E49D0AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3895FAC4-FCC6-4110-984E-DCEBA428B0AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="50">
   <si>
     <t>Date</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>Add Memory Control 1</t>
+  </si>
+  <si>
+    <t>Add ROM 1</t>
   </si>
 </sst>
 </file>
@@ -524,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,7 +637,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D40" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D41" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1391,6 +1394,30 @@
       </c>
       <c r="G40" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C41" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D41" s="3">
+        <f t="shared" si="0"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G41" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create ROM 2 IP Core
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3895FAC4-FCC6-4110-984E-DCEBA428B0AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CA9076-A7EE-4740-9285-A282A971600B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>Add ROM 1</t>
+  </si>
+  <si>
+    <t>ROM 2</t>
+  </si>
+  <si>
+    <t>Create IP Core</t>
   </si>
 </sst>
 </file>
@@ -527,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,7 +643,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D41" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D42" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1418,6 +1424,30 @@
       </c>
       <c r="G41" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C42" s="5">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G42" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create ROM 2 testbench
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CA9076-A7EE-4740-9285-A282A971600B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4656A683-79B0-46F8-A0FE-C1DBF4EFA74D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -533,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,7 +643,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D42" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D43" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1448,6 +1448,27 @@
       </c>
       <c r="G42" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="5">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="C43" s="5">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D43" s="3">
+        <f t="shared" si="0"/>
+        <v>3.4722222222222099E-3</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add architecture and testbench of Memory Control 2
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4656A683-79B0-46F8-A0FE-C1DBF4EFA74D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFDBB2A-CC88-4B98-A7CE-1BE2E4AEDC50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>Create IP Core</t>
+  </si>
+  <si>
+    <t>Mem Ctrl 2</t>
   </si>
 </sst>
 </file>
@@ -533,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,7 +646,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D43" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D44" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1469,6 +1472,27 @@
       </c>
       <c r="F43" s="6" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="5">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="C44" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D44" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Memory Control 2 and ROM 2 to VGA Top
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFDBB2A-CC88-4B98-A7CE-1BE2E4AEDC50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D3A011-597C-431F-B3F2-A062F38420FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="54">
   <si>
     <t>Date</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>Mem Ctrl 2</t>
+  </si>
+  <si>
+    <t>Add Memory Control 2 and ROM 2</t>
   </si>
 </sst>
 </file>
@@ -536,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,7 +649,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D44" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D45" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1493,6 +1496,30 @@
       </c>
       <c r="F44" s="6" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C45" s="5">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D45" s="3">
+        <f t="shared" si="0"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G45" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add packages for constant
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D3A011-597C-431F-B3F2-A062F38420FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA14828B-9C53-4FD5-8DAD-63CEE871EAD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -195,6 +195,12 @@
   </si>
   <si>
     <t>Add Memory Control 2 and ROM 2</t>
+  </si>
+  <si>
+    <t>Add packages for simulation</t>
+  </si>
+  <si>
+    <t>Project</t>
   </si>
 </sst>
 </file>
@@ -539,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,7 +655,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D45" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D46" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1520,6 +1526,30 @@
       </c>
       <c r="G45" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="5">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="C46" s="5">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="D46" s="3">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G46" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use packages in IO debounce testbench
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA14828B-9C53-4FD5-8DAD-63CEE871EAD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D36989F-E52C-4E94-B850-8D9C95DDCB19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t>Project</t>
+  </si>
+  <si>
+    <t>Improve Testbench</t>
+  </si>
+  <si>
+    <t>Use added packages</t>
   </si>
 </sst>
 </file>
@@ -545,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,7 +661,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D46" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D47" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1551,6 +1557,33 @@
       <c r="G46" t="s">
         <v>54</v>
       </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" s="5">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="C47" s="5">
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="D47" s="3">
+        <f t="shared" si="0"/>
+        <v>2.7777777777777679E-2</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Move object with button press
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D36989F-E52C-4E94-B850-8D9C95DDCB19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF73DCCC-4379-448A-8DA5-333D39D148F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t>Use added packages</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>Add button move support</t>
   </si>
 </sst>
 </file>
@@ -554,7 +560,7 @@
   <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,7 +667,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D47" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D48" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1580,6 +1586,30 @@
       </c>
       <c r="G47" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="5">
+        <v>0.65625</v>
+      </c>
+      <c r="C48" s="5">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="D48" s="3">
+        <f t="shared" si="0"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G48" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add packages to Memory Control 1
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF73DCCC-4379-448A-8DA5-333D39D148F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D1B7EA-B440-4E6D-88EC-F4EDAFEF5575}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t>Add button move support</t>
+  </si>
+  <si>
+    <t>6.4.2020</t>
+  </si>
+  <si>
+    <t>Add packages</t>
   </si>
 </sst>
 </file>
@@ -559,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +673,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D48" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D49" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1612,7 +1618,31 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C49" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D49" s="3">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G49" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D52" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add packages to Memory Control 2
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D1B7EA-B440-4E6D-88EC-F4EDAFEF5575}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892B912A-650A-48A3-9431-BD20B7AC664B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -566,7 +566,7 @@
   <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +673,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D49" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D50" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1639,6 +1639,30 @@
         <v>31</v>
       </c>
       <c r="G49" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C50" s="5">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="D50" s="3">
+        <f t="shared" si="0"/>
+        <v>1.3888888888888951E-2</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G50" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add packages to Pattern Gen 2
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892B912A-650A-48A3-9431-BD20B7AC664B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0800C10E-003F-4477-AEC2-CDA4153554F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="63">
   <si>
     <t>Date</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>Add packages</t>
+  </si>
+  <si>
+    <t>Imrpove Code</t>
   </si>
 </sst>
 </file>
@@ -566,7 +569,7 @@
   <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +676,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D50" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D52" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1666,8 +1669,53 @@
         <v>61</v>
       </c>
     </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" s="5">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="C51" s="5">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="D51" s="3">
+        <f t="shared" si="0"/>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G51" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D52" s="5"/>
+      <c r="A52" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" s="5">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="C52" s="5">
+        <v>0.5625</v>
+      </c>
+      <c r="D52" s="5">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G52" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Add packages to VGA Control
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0800C10E-003F-4477-AEC2-CDA4153554F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6039C3E4-C695-4DB2-A44F-27DCDAA930FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -219,9 +219,6 @@
   </si>
   <si>
     <t>Add packages</t>
-  </si>
-  <si>
-    <t>Imrpove Code</t>
   </si>
 </sst>
 </file>
@@ -566,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,7 +673,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D52" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D54" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1711,9 +1708,57 @@
         <v>19</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="G52" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" s="5">
+        <v>0.5625</v>
+      </c>
+      <c r="C53" s="5">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="D53" s="3">
+        <f t="shared" si="0"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G53" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" s="5">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="C54" s="5">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D54" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G54" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add packages to VGA Top
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6039C3E4-C695-4DB2-A44F-27DCDAA930FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907F8796-5685-4341-8961-BB8908DFAE87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -563,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +673,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D54" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D57" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1759,6 +1759,78 @@
         <v>31</v>
       </c>
       <c r="G54" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B55" s="5">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C55" s="5">
+        <v>0.58680555555555558</v>
+      </c>
+      <c r="D55" s="3">
+        <f t="shared" si="0"/>
+        <v>3.4722222222222099E-3</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G55" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" s="5">
+        <v>0.58680555555555558</v>
+      </c>
+      <c r="C56" s="5">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="D56" s="3">
+        <f t="shared" si="0"/>
+        <v>3.4722222222222099E-3</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G56" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" s="5">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="C57" s="5">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="D57" s="3">
+        <f t="shared" si="0"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G57" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implementation of desgin into Vivado and download on board
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907F8796-5685-4341-8961-BB8908DFAE87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431CD998-07B6-4675-99EA-14A689B74425}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="64">
   <si>
     <t>Date</t>
   </si>
@@ -219,6 +219,12 @@
   </si>
   <si>
     <t>Add packages</t>
+  </si>
+  <si>
+    <t>7.4.2020</t>
+  </si>
+  <si>
+    <t>Implementation</t>
   </si>
 </sst>
 </file>
@@ -563,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +679,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D57" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D58" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1833,6 +1839,30 @@
       <c r="G57" t="s">
         <v>61</v>
       </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C58" s="5">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D58" s="3">
+        <f t="shared" si="0"/>
+        <v>0.14583333333333337</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D61" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Final documentation of files
</commit_message>
<xml_diff>
--- a/doc/Time Record.xlsx
+++ b/doc/Time Record.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\chd\vga_controller\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Technikum\chd\vga_controller\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431CD998-07B6-4675-99EA-14A689B74425}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703FEE8F-A69F-4706-982B-89AC52F86798}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="68">
   <si>
     <t>Date</t>
   </si>
@@ -225,6 +223,18 @@
   </si>
   <si>
     <t>Implementation</t>
+  </si>
+  <si>
+    <t>14.4.2020</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Last documentation of files</t>
+  </si>
+  <si>
+    <t>Write documentation PDF</t>
   </si>
 </sst>
 </file>
@@ -291,7 +301,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -572,10 +582,10 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="25.140625" customWidth="1"/>
     <col min="6" max="6" width="42.5703125" customWidth="1"/>
@@ -679,7 +689,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D58" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D60" si="0">C5-B5</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1859,6 +1869,54 @@
       </c>
       <c r="F58" s="6" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="C59" s="5">
+        <v>0.40625</v>
+      </c>
+      <c r="D59" s="3">
+        <f t="shared" si="0"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G59" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B60" s="5">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C60" s="5">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D60" s="3">
+        <f t="shared" si="0"/>
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G60" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>